<commit_message>
rename sheet names to template name
remove the "naming convention"
</commit_message>
<xml_diff>
--- a/templates/dataplant/1SPL01_plants.xlsx
+++ b/templates/dataplant/1SPL01_plants.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/github/nfdi4plants/Swate-templates/templates/dataplant/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6F4249-274E-2946-AD38-25497FC1E103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0802DC5-DB85-FE46-BF67-B506B6D06577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25020" yWindow="-21100" windowWidth="19200" windowHeight="21100" activeTab="2" xr2:uid="{2D1671A6-E5E6-4E90-817E-C23847CD9BD1}"/>
+    <workbookView xWindow="-25000" yWindow="-21100" windowWidth="19200" windowHeight="21100" xr2:uid="{2D1671A6-E5E6-4E90-817E-C23847CD9BD1}"/>
   </bookViews>
   <sheets>
-    <sheet name="1SPL01_plants" sheetId="1" r:id="rId1"/>
+    <sheet name="plant_growth" sheetId="1" r:id="rId1"/>
     <sheet name="SwateTemplateMetadata" sheetId="3" r:id="rId2"/>
     <sheet name="METABOLIGHTS_METABOLOMICS" sheetId="5" r:id="rId3"/>
     <sheet name="BIOSAMPLE_PLANTS" sheetId="6" r:id="rId4"/>
@@ -2590,7 +2590,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8916BF-D1BA-4E62-B448-EB2F6971FAFB}">
   <dimension ref="A1:ER7"/>
   <sheetViews>
-    <sheetView topLeftCell="AF1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4161,7 +4161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C806736B-09AD-44FE-B8F6-60FEE51F74DE}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
@@ -4506,7 +4506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
[test] adding unique values for protocol type
</commit_message>
<xml_diff>
--- a/templates/dataplant/1SPL01_plants.xlsx
+++ b/templates/dataplant/1SPL01_plants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/github/nfdi4plants/SWATE_templates/templates/dataplant/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A06ACAA-B7A6-1548-B4B8-6BA76BB4BBC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791D0011-C61B-AE44-A3F3-26BE6AABE2A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -198,7 +198,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="540">
   <si>
     <t>Source Name</t>
   </si>
@@ -2792,7 +2792,7 @@
   <dimension ref="A1:EV7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B7" sqref="B7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3633,9 +3633,15 @@
       <c r="EV2" s="3"/>
     </row>
     <row r="3" spans="1:152" x14ac:dyDescent="0.2">
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
+      <c r="B3" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>154</v>
+      </c>
       <c r="E3" s="19"/>
       <c r="F3" t="s">
         <v>180</v>
@@ -3830,9 +3836,15 @@
       <c r="EV3" s="3"/>
     </row>
     <row r="4" spans="1:152" x14ac:dyDescent="0.2">
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
+      <c r="B4" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>154</v>
+      </c>
       <c r="E4" s="19"/>
       <c r="F4" t="s">
         <v>191</v>
@@ -4003,9 +4015,15 @@
       <c r="EV4" s="3"/>
     </row>
     <row r="5" spans="1:152" x14ac:dyDescent="0.2">
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
+      <c r="B5" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>154</v>
+      </c>
       <c r="E5" s="19"/>
       <c r="F5" t="s">
         <v>200</v>
@@ -4140,9 +4158,15 @@
       <c r="EV5" s="3"/>
     </row>
     <row r="6" spans="1:152" x14ac:dyDescent="0.2">
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
+      <c r="B6" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>154</v>
+      </c>
       <c r="E6" s="19"/>
       <c r="F6" t="s">
         <v>202</v>
@@ -4268,9 +4292,15 @@
       <c r="EV6" s="3"/>
     </row>
     <row r="7" spans="1:152" x14ac:dyDescent="0.2">
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
+      <c r="B7" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>154</v>
+      </c>
       <c r="E7" s="19"/>
       <c r="F7" t="s">
         <v>203</v>

</xml_diff>

<commit_message>
[test] unique protocol REF values
</commit_message>
<xml_diff>
--- a/templates/dataplant/1SPL01_plants.xlsx
+++ b/templates/dataplant/1SPL01_plants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/github/nfdi4plants/SWATE_templates/templates/dataplant/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791D0011-C61B-AE44-A3F3-26BE6AABE2A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4242559-CF84-E943-9E92-B7EC37215F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -198,7 +198,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="541">
   <si>
     <t>Source Name</t>
   </si>
@@ -1830,6 +1830,9 @@
   </si>
   <si>
     <t>Parameter [sample collection date]</t>
+  </si>
+  <si>
+    <t>plant-growth.txt</t>
   </si>
 </sst>
 </file>
@@ -2792,7 +2795,7 @@
   <dimension ref="A1:EV7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:D7"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3418,7 +3421,9 @@
       <c r="D2" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="E2" s="19"/>
+      <c r="E2" s="19" t="s">
+        <v>540</v>
+      </c>
       <c r="F2" t="s">
         <v>155</v>
       </c>
@@ -3642,7 +3647,9 @@
       <c r="D3" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="E3" s="19"/>
+      <c r="E3" s="19" t="s">
+        <v>540</v>
+      </c>
       <c r="F3" t="s">
         <v>180</v>
       </c>
@@ -3845,7 +3852,9 @@
       <c r="D4" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="E4" s="19"/>
+      <c r="E4" s="19" t="s">
+        <v>540</v>
+      </c>
       <c r="F4" t="s">
         <v>191</v>
       </c>
@@ -4024,7 +4033,9 @@
       <c r="D5" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="E5" s="19"/>
+      <c r="E5" s="19" t="s">
+        <v>540</v>
+      </c>
       <c r="F5" t="s">
         <v>200</v>
       </c>
@@ -4167,7 +4178,9 @@
       <c r="D6" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="E6" s="19"/>
+      <c r="E6" s="19" t="s">
+        <v>540</v>
+      </c>
       <c r="F6" t="s">
         <v>202</v>
       </c>
@@ -4301,7 +4314,9 @@
       <c r="D7" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="E7" s="19"/>
+      <c r="E7" s="19" t="s">
+        <v>540</v>
+      </c>
       <c r="F7" t="s">
         <v>203</v>
       </c>

</xml_diff>